<commit_message>
Yilun updated Aug 1st
</commit_message>
<xml_diff>
--- a/gensim_食品_地点_店家归类/地点/data/places.xlsx
+++ b/gensim_食品_地点_店家归类/地点/data/places.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
   <si>
     <t>地区描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,10 +49,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>学校北门附近</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>一附属</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -257,10 +253,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>学校附近</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>白堤路/风荷园</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -269,18 +261,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>体院北</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>南开/天大校区</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>妇产科医院</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>西康路沿线</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -418,6 +402,14 @@
   </si>
   <si>
     <t>庆丰路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学校北门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校内</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -746,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -757,23 +749,23 @@
     <col min="2" max="2" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -781,7 +773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -789,23 +781,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -813,7 +805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -821,141 +813,111 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="C15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" t="s">
-        <v>54</v>
-      </c>
-      <c r="J15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -963,7 +925,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -971,23 +933,23 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -995,7 +957,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1003,7 +965,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1011,7 +973,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1019,7 +981,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1027,7 +989,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1035,23 +997,23 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1059,55 +1021,55 @@
         <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1115,319 +1077,319 @@
         <v>33</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>